<commit_message>
versao utilizando somente selenium
</commit_message>
<xml_diff>
--- a/isencao.xlsx
+++ b/isencao.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>pdv</t>
   </si>
@@ -33,7 +33,13 @@
     <t>525-890-390</t>
   </si>
   <si>
-    <t xml:space="preserve">526-622-584 </t>
+    <t>dataisencao</t>
+  </si>
+  <si>
+    <t>526-622-584</t>
+  </si>
+  <si>
+    <t>24/05/2999</t>
   </si>
 </sst>
 </file>
@@ -77,7 +83,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -86,6 +92,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,14 +381,15 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -389,7 +402,9 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -398,19 +413,25 @@
       <c r="B2" s="1">
         <v>1360</v>
       </c>
-      <c r="C2" s="1">
-        <v>69.900000000000006</v>
+      <c r="C2" s="4">
+        <v>99.9</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
         <v>1360</v>
       </c>
-      <c r="C3" s="1">
-        <v>99.9</v>
+      <c r="C3" s="4">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>